<commit_message>
changing data processing pipeline for freebase
</commit_message>
<xml_diff>
--- a/data/freebase/dumb_records.xlsx
+++ b/data/freebase/dumb_records.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J69"/>
+  <dimension ref="A1:K69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,6 +476,11 @@
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
+          <t>answer_mid</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
           <t>relation_span</t>
         </is>
       </c>
@@ -504,7 +509,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>fb:m.02015n</t>
+          <t>fb:m.0hqrhvc</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -523,6 +528,11 @@
         </is>
       </c>
       <c r="J2" t="inlineStr">
+        <is>
+          <t>fb:m.0hqrhvc</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
         <is>
           <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -552,7 +562,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>fb:m.0fvs6bh</t>
+          <t>fb:m.0qg9698</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -571,6 +581,11 @@
         </is>
       </c>
       <c r="J3" t="inlineStr">
+        <is>
+          <t>fb:m.0qg9698</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -600,7 +615,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>fb:m.09jd9nh</t>
+          <t>fb:m.0y9w_wv</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -619,6 +634,11 @@
         </is>
       </c>
       <c r="J4" t="inlineStr">
+        <is>
+          <t>fb:m.0y9w_wv</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -648,7 +668,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>fb:m.0fdjb</t>
+          <t>fb:m.02ww_qc</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -667,6 +687,11 @@
         </is>
       </c>
       <c r="J5" t="inlineStr">
+        <is>
+          <t>fb:m.02ww_qc</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -696,7 +721,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>fb:m.06zpsmp</t>
+          <t>fb:m.03yvtl5</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -715,6 +740,11 @@
         </is>
       </c>
       <c r="J6" t="inlineStr">
+        <is>
+          <t>fb:m.03yvtl5</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -744,7 +774,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>fb:m.0l14g2</t>
+          <t>fb:m.01k0677</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -763,6 +793,11 @@
         </is>
       </c>
       <c r="J7" t="inlineStr">
+        <is>
+          <t>fb:m.01k0677</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -792,7 +827,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>fb:m.0jtdp</t>
+          <t>fb:m.0gw7q_r</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -811,6 +846,11 @@
         </is>
       </c>
       <c r="J8" t="inlineStr">
+        <is>
+          <t>fb:m.0gw7q_r</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -840,7 +880,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>fb:m.0cn6d25</t>
+          <t>fb:m.0319xp</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -859,6 +899,11 @@
         </is>
       </c>
       <c r="J9" t="inlineStr">
+        <is>
+          <t>fb:m.0319xp</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -888,7 +933,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>fb:m.0fngy</t>
+          <t>fb:m.0jw1qp1</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -907,6 +952,11 @@
         </is>
       </c>
       <c r="J10" t="inlineStr">
+        <is>
+          <t>fb:m.0jw1qp1</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -936,7 +986,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>fb:m.010cbj4</t>
+          <t>fb:m.0g71sbj</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -955,6 +1005,11 @@
         </is>
       </c>
       <c r="J11" t="inlineStr">
+        <is>
+          <t>fb:m.0g71sbj</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -984,7 +1039,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>fb:m.05b4w</t>
+          <t>fb:m.0z85h70</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -1003,6 +1058,11 @@
         </is>
       </c>
       <c r="J12" t="inlineStr">
+        <is>
+          <t>fb:m.0z85h70</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -1032,7 +1092,7 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>fb:m.055kfg</t>
+          <t>fb:m.0nn66b_</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -1051,6 +1111,11 @@
         </is>
       </c>
       <c r="J13" t="inlineStr">
+        <is>
+          <t>fb:m.0nn66b_</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -1080,7 +1145,7 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>fb:m.02jbfk</t>
+          <t>fb:m.0fr47rb</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
@@ -1099,6 +1164,11 @@
         </is>
       </c>
       <c r="J14" t="inlineStr">
+        <is>
+          <t>fb:m.0fr47rb</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -1128,7 +1198,7 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>fb:m.02kjb_</t>
+          <t>fb:m.0hqtlv8</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
@@ -1147,6 +1217,11 @@
         </is>
       </c>
       <c r="J15" t="inlineStr">
+        <is>
+          <t>fb:m.0hqtlv8</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
         <is>
           <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -1176,7 +1251,7 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>fb:m.02jbfk</t>
+          <t>fb:m.0f8w6q8</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -1195,6 +1270,11 @@
         </is>
       </c>
       <c r="J16" t="inlineStr">
+        <is>
+          <t>fb:m.0f8w6q8</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -1224,7 +1304,7 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>fb:m.01xryvt</t>
+          <t>fb:m.01wy9d</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
@@ -1243,6 +1323,11 @@
         </is>
       </c>
       <c r="J17" t="inlineStr">
+        <is>
+          <t>fb:m.01wy9d</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
         <is>
           <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -1272,7 +1357,7 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>fb:m.0l14g2</t>
+          <t>fb:m.05ssss_</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
@@ -1291,6 +1376,11 @@
         </is>
       </c>
       <c r="J18" t="inlineStr">
+        <is>
+          <t>fb:m.05ssss_</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
         <is>
           <t>[0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -1320,7 +1410,7 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>fb:m.0jfb0</t>
+          <t>fb:m.05n0276</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
@@ -1339,6 +1429,11 @@
         </is>
       </c>
       <c r="J19" t="inlineStr">
+        <is>
+          <t>fb:m.05n0276</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -1368,7 +1463,7 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>fb:m.03y9cqy</t>
+          <t>fb:m.02h664x</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
@@ -1387,6 +1482,11 @@
         </is>
       </c>
       <c r="J20" t="inlineStr">
+        <is>
+          <t>fb:m.02h664x</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -1416,7 +1516,7 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>fb:m.01_7r6</t>
+          <t>fb:m.0hqr7sx</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
@@ -1435,6 +1535,11 @@
         </is>
       </c>
       <c r="J21" t="inlineStr">
+        <is>
+          <t>fb:m.0hqr7sx</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
         <is>
           <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -1464,7 +1569,7 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>fb:m.088q4</t>
+          <t>fb:m.0j3wpr6</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
@@ -1483,6 +1588,11 @@
         </is>
       </c>
       <c r="J22" t="inlineStr">
+        <is>
+          <t>fb:m.0j3wpr6</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -1512,7 +1622,7 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>fb:m.0137n0</t>
+          <t>fb:m.058mwwp</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
@@ -1531,6 +1641,11 @@
         </is>
       </c>
       <c r="J23" t="inlineStr">
+        <is>
+          <t>fb:m.058mwwp</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -1560,7 +1675,7 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>fb:m.03npn</t>
+          <t>fb:m.0x17tvr</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
@@ -1579,6 +1694,11 @@
         </is>
       </c>
       <c r="J24" t="inlineStr">
+        <is>
+          <t>fb:m.0x17tvr</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -1608,7 +1728,7 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>fb:m.0lj8m</t>
+          <t>fb:m.02h7hyr</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
@@ -1627,6 +1747,11 @@
         </is>
       </c>
       <c r="J25" t="inlineStr">
+        <is>
+          <t>fb:m.02h7hyr</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -1656,7 +1781,7 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>fb:m.01vsy7t</t>
+          <t>fb:m.0zmpz4</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
@@ -1675,6 +1800,11 @@
         </is>
       </c>
       <c r="J26" t="inlineStr">
+        <is>
+          <t>fb:m.0zmpz4</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -1704,7 +1834,7 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>fb:m.0fr432l</t>
+          <t>fb:m.0g1vb16</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
@@ -1723,6 +1853,11 @@
         </is>
       </c>
       <c r="J27" t="inlineStr">
+        <is>
+          <t>fb:m.0g1vb16</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -1752,7 +1887,7 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>fb:m.015qv41</t>
+          <t>fb:m.033g8n3</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
@@ -1771,6 +1906,11 @@
         </is>
       </c>
       <c r="J28" t="inlineStr">
+        <is>
+          <t>fb:m.033g8n3</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -1800,7 +1940,7 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>fb:m.01lzhcr</t>
+          <t>fb:m.0nm3chn</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
@@ -1819,6 +1959,11 @@
         </is>
       </c>
       <c r="J29" t="inlineStr">
+        <is>
+          <t>fb:m.0nm3chn</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -1848,7 +1993,7 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>fb:m.0dd9p</t>
+          <t>fb:m.02qkdzb</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
@@ -1867,6 +2012,11 @@
         </is>
       </c>
       <c r="J30" t="inlineStr">
+        <is>
+          <t>fb:m.02qkdzb</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -1896,7 +2046,7 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>fb:m.054xs9</t>
+          <t>fb:m.0b44bzz</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
@@ -1915,6 +2065,11 @@
         </is>
       </c>
       <c r="J31" t="inlineStr">
+        <is>
+          <t>fb:m.0b44bzz</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -1944,7 +2099,7 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>fb:m.02lx2r</t>
+          <t>fb:m.07kg0mk</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
@@ -1963,6 +2118,11 @@
         </is>
       </c>
       <c r="J32" t="inlineStr">
+        <is>
+          <t>fb:m.07kg0mk</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -1992,7 +2152,7 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>fb:m.01vrz41</t>
+          <t>fb:m.0d_bb4h</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
@@ -2011,6 +2171,11 @@
         </is>
       </c>
       <c r="J33" t="inlineStr">
+        <is>
+          <t>fb:m.0d_bb4h</t>
+        </is>
+      </c>
+      <c r="K33" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -2040,7 +2205,7 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>fb:m.01vyymq</t>
+          <t>fb:m.013f7rh</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
@@ -2059,6 +2224,11 @@
         </is>
       </c>
       <c r="J34" t="inlineStr">
+        <is>
+          <t>fb:m.013f7rh</t>
+        </is>
+      </c>
+      <c r="K34" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -2088,7 +2258,7 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>fb:m.0g7zq1h</t>
+          <t>fb:m.0rtydgw</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
@@ -2107,6 +2277,11 @@
         </is>
       </c>
       <c r="J35" t="inlineStr">
+        <is>
+          <t>fb:m.0rtydgw</t>
+        </is>
+      </c>
+      <c r="K35" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -2136,7 +2311,7 @@
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>fb:m.01_9c1</t>
+          <t>fb:m.0jbctxx</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
@@ -2155,6 +2330,11 @@
         </is>
       </c>
       <c r="J36" t="inlineStr">
+        <is>
+          <t>fb:m.0jbctxx</t>
+        </is>
+      </c>
+      <c r="K36" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -2184,7 +2364,7 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>fb:m.06vqn8</t>
+          <t>fb:m.0hqskn0</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
@@ -2203,6 +2383,11 @@
         </is>
       </c>
       <c r="J37" t="inlineStr">
+        <is>
+          <t>fb:m.0hqskn0</t>
+        </is>
+      </c>
+      <c r="K37" t="inlineStr">
         <is>
           <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -2232,7 +2417,7 @@
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>fb:m.02jbfk</t>
+          <t>fb:m.0f5n8xz</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
@@ -2251,6 +2436,11 @@
         </is>
       </c>
       <c r="J38" t="inlineStr">
+        <is>
+          <t>fb:m.0f5n8xz</t>
+        </is>
+      </c>
+      <c r="K38" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -2280,7 +2470,7 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>fb:m.0kyqg6_</t>
+          <t>fb:m.01pvj8</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
@@ -2299,6 +2489,11 @@
         </is>
       </c>
       <c r="J39" t="inlineStr">
+        <is>
+          <t>fb:m.01pvj8</t>
+        </is>
+      </c>
+      <c r="K39" t="inlineStr">
         <is>
           <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -2328,7 +2523,7 @@
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>fb:m.0jwydj2</t>
+          <t>fb:m.02h664x</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
@@ -2347,6 +2542,11 @@
         </is>
       </c>
       <c r="J40" t="inlineStr">
+        <is>
+          <t>fb:m.02h664x</t>
+        </is>
+      </c>
+      <c r="K40" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -2376,7 +2576,7 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>fb:m.09c7w0</t>
+          <t>fb:m.0byd4y8</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
@@ -2395,6 +2595,11 @@
         </is>
       </c>
       <c r="J41" t="inlineStr">
+        <is>
+          <t>fb:m.0byd4y8</t>
+        </is>
+      </c>
+      <c r="K41" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -2424,7 +2629,7 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>fb:m.03fjv0m</t>
+          <t>fb:m.0mkvdy4</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
@@ -2443,6 +2648,11 @@
         </is>
       </c>
       <c r="J42" t="inlineStr">
+        <is>
+          <t>fb:m.0mkvdy4</t>
+        </is>
+      </c>
+      <c r="K42" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -2472,7 +2682,7 @@
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>fb:m.02kjb_</t>
+          <t>fb:m.0hqrcx6</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
@@ -2491,6 +2701,11 @@
         </is>
       </c>
       <c r="J43" t="inlineStr">
+        <is>
+          <t>fb:m.0hqrcx6</t>
+        </is>
+      </c>
+      <c r="K43" t="inlineStr">
         <is>
           <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -2520,7 +2735,7 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>fb:m.07vcwc</t>
+          <t>fb:m.05dbwcp</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
@@ -2539,6 +2754,11 @@
         </is>
       </c>
       <c r="J44" t="inlineStr">
+        <is>
+          <t>fb:m.05dbwcp</t>
+        </is>
+      </c>
+      <c r="K44" t="inlineStr">
         <is>
           <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -2568,7 +2788,7 @@
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>fb:m.01b86_</t>
+          <t>fb:m.0hqrs1d</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
@@ -2587,6 +2807,11 @@
         </is>
       </c>
       <c r="J45" t="inlineStr">
+        <is>
+          <t>fb:m.0hqrs1d</t>
+        </is>
+      </c>
+      <c r="K45" t="inlineStr">
         <is>
           <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -2616,7 +2841,7 @@
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>fb:m.0bqmg2</t>
+          <t>fb:m.02kc1x8</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
@@ -2635,6 +2860,11 @@
         </is>
       </c>
       <c r="J46" t="inlineStr">
+        <is>
+          <t>fb:m.02kc1x8</t>
+        </is>
+      </c>
+      <c r="K46" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -2664,7 +2894,7 @@
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>fb:m.0gjc9wy</t>
+          <t>fb:m.02h664x</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
@@ -2683,6 +2913,11 @@
         </is>
       </c>
       <c r="J47" t="inlineStr">
+        <is>
+          <t>fb:m.02h664x</t>
+        </is>
+      </c>
+      <c r="K47" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -2712,7 +2947,7 @@
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>fb:m.0xz_h</t>
+          <t>fb:m.0zgl46r</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
@@ -2731,6 +2966,11 @@
         </is>
       </c>
       <c r="J48" t="inlineStr">
+        <is>
+          <t>fb:m.0zgl46r</t>
+        </is>
+      </c>
+      <c r="K48" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -2760,7 +3000,7 @@
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>fb:m.041104g</t>
+          <t>fb:m.0kpck1k</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
@@ -2779,6 +3019,11 @@
         </is>
       </c>
       <c r="J49" t="inlineStr">
+        <is>
+          <t>fb:m.0kpck1k</t>
+        </is>
+      </c>
+      <c r="K49" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -2808,7 +3053,7 @@
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>fb:m.0238mf</t>
+          <t>fb:m.0_jqh5j</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
@@ -2827,6 +3072,11 @@
         </is>
       </c>
       <c r="J50" t="inlineStr">
+        <is>
+          <t>fb:m.0_jqh5j</t>
+        </is>
+      </c>
+      <c r="K50" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -2856,7 +3106,7 @@
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>fb:m.0dr846n</t>
+          <t>fb:m.0km51t_</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
@@ -2875,6 +3125,11 @@
         </is>
       </c>
       <c r="J51" t="inlineStr">
+        <is>
+          <t>fb:m.0km51t_</t>
+        </is>
+      </c>
+      <c r="K51" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -2904,7 +3159,7 @@
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>fb:m.0sl5hgc</t>
+          <t>fb:m.0v48dg8</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
@@ -2923,6 +3178,11 @@
         </is>
       </c>
       <c r="J52" t="inlineStr">
+        <is>
+          <t>fb:m.0v48dg8</t>
+        </is>
+      </c>
+      <c r="K52" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -2952,7 +3212,7 @@
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>fb:m.02kjb_</t>
+          <t>fb:m.0hqth1v</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
@@ -2971,6 +3231,11 @@
         </is>
       </c>
       <c r="J53" t="inlineStr">
+        <is>
+          <t>fb:m.0hqth1v</t>
+        </is>
+      </c>
+      <c r="K53" t="inlineStr">
         <is>
           <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -3000,7 +3265,7 @@
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>fb:m.031rm1</t>
+          <t>fb:m.0k33swc</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
@@ -3019,6 +3284,11 @@
         </is>
       </c>
       <c r="J54" t="inlineStr">
+        <is>
+          <t>fb:m.0k33swc</t>
+        </is>
+      </c>
+      <c r="K54" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -3048,7 +3318,7 @@
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>fb:m.03wrrj</t>
+          <t>fb:m.06hsptf</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
@@ -3067,6 +3337,11 @@
         </is>
       </c>
       <c r="J55" t="inlineStr">
+        <is>
+          <t>fb:m.06hsptf</t>
+        </is>
+      </c>
+      <c r="K55" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -3096,7 +3371,7 @@
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>fb:m.02c3_1</t>
+          <t>fb:m.04w2yxm</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
@@ -3115,6 +3390,11 @@
         </is>
       </c>
       <c r="J56" t="inlineStr">
+        <is>
+          <t>fb:m.04w2yxm</t>
+        </is>
+      </c>
+      <c r="K56" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -3144,7 +3424,7 @@
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>fb:m.06f3l</t>
+          <t>fb:m.05h4n_p</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
@@ -3163,6 +3443,11 @@
         </is>
       </c>
       <c r="J57" t="inlineStr">
+        <is>
+          <t>fb:m.05h4n_p</t>
+        </is>
+      </c>
+      <c r="K57" t="inlineStr">
         <is>
           <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -3192,7 +3477,7 @@
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>fb:m.01j4cg_</t>
+          <t>fb:m.0r4l5d</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
@@ -3211,6 +3496,11 @@
         </is>
       </c>
       <c r="J58" t="inlineStr">
+        <is>
+          <t>fb:m.0r4l5d</t>
+        </is>
+      </c>
+      <c r="K58" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -3240,7 +3530,7 @@
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>fb:m.02_fj</t>
+          <t>fb:m.0fjg6cy</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
@@ -3259,6 +3549,11 @@
         </is>
       </c>
       <c r="J59" t="inlineStr">
+        <is>
+          <t>fb:m.0fjg6cy</t>
+        </is>
+      </c>
+      <c r="K59" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -3288,7 +3583,7 @@
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>fb:m.05zppz</t>
+          <t>fb:m.0h81j6h</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
@@ -3307,6 +3602,11 @@
         </is>
       </c>
       <c r="J60" t="inlineStr">
+        <is>
+          <t>fb:m.0h81j6h</t>
+        </is>
+      </c>
+      <c r="K60" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -3336,7 +3636,7 @@
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>fb:m.0q01m</t>
+          <t>fb:m.02kbxdm</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
@@ -3355,6 +3655,11 @@
         </is>
       </c>
       <c r="J61" t="inlineStr">
+        <is>
+          <t>fb:m.02kbxdm</t>
+        </is>
+      </c>
+      <c r="K61" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -3384,7 +3689,7 @@
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>fb:m.056vv</t>
+          <t>fb:m.0cz7_3h</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
@@ -3403,6 +3708,11 @@
         </is>
       </c>
       <c r="J62" t="inlineStr">
+        <is>
+          <t>fb:m.0cz7_3h</t>
+        </is>
+      </c>
+      <c r="K62" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -3432,7 +3742,7 @@
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>fb:m.01k5j1d</t>
+          <t>fb:m.01k5hzy</t>
         </is>
       </c>
       <c r="G63" t="inlineStr">
@@ -3451,6 +3761,11 @@
         </is>
       </c>
       <c r="J63" t="inlineStr">
+        <is>
+          <t>fb:m.01k5hzy</t>
+        </is>
+      </c>
+      <c r="K63" t="inlineStr">
         <is>
           <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -3480,7 +3795,7 @@
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>fb:m.02hjn4</t>
+          <t>fb:m.06k50f</t>
         </is>
       </c>
       <c r="G64" t="inlineStr">
@@ -3499,6 +3814,11 @@
         </is>
       </c>
       <c r="J64" t="inlineStr">
+        <is>
+          <t>fb:m.06k50f</t>
+        </is>
+      </c>
+      <c r="K64" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -3528,7 +3848,7 @@
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>fb:m.039kc6q</t>
+          <t>fb:m.0ls67qg</t>
         </is>
       </c>
       <c r="G65" t="inlineStr">
@@ -3547,6 +3867,11 @@
         </is>
       </c>
       <c r="J65" t="inlineStr">
+        <is>
+          <t>fb:m.0ls67qg</t>
+        </is>
+      </c>
+      <c r="K65" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -3576,7 +3901,7 @@
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>fb:m.0sjwsl</t>
+          <t>fb:m.01npl51</t>
         </is>
       </c>
       <c r="G66" t="inlineStr">
@@ -3595,6 +3920,11 @@
         </is>
       </c>
       <c r="J66" t="inlineStr">
+        <is>
+          <t>fb:m.01npl51</t>
+        </is>
+      </c>
+      <c r="K66" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -3624,7 +3954,7 @@
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>fb:m.0674bs</t>
+          <t>fb:m.03jhpgp</t>
         </is>
       </c>
       <c r="G67" t="inlineStr">
@@ -3643,6 +3973,11 @@
         </is>
       </c>
       <c r="J67" t="inlineStr">
+        <is>
+          <t>fb:m.03jhpgp</t>
+        </is>
+      </c>
+      <c r="K67" t="inlineStr">
         <is>
           <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -3672,7 +4007,7 @@
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>fb:m.02kjb_</t>
+          <t>fb:m.0hqv1cb</t>
         </is>
       </c>
       <c r="G68" t="inlineStr">
@@ -3691,6 +4026,11 @@
         </is>
       </c>
       <c r="J68" t="inlineStr">
+        <is>
+          <t>fb:m.0hqv1cb</t>
+        </is>
+      </c>
+      <c r="K68" t="inlineStr">
         <is>
           <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -3720,7 +4060,7 @@
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>fb:m.0ggq0m</t>
+          <t>fb:m.04634rs</t>
         </is>
       </c>
       <c r="G69" t="inlineStr">
@@ -3739,6 +4079,11 @@
         </is>
       </c>
       <c r="J69" t="inlineStr">
+        <is>
+          <t>fb:m.04634rs</t>
+        </is>
+      </c>
+      <c r="K69" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>

</xml_diff>

<commit_message>
adding relation type to freebase data
</commit_message>
<xml_diff>
--- a/data/freebase/dumb_records.xlsx
+++ b/data/freebase/dumb_records.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K69"/>
+  <dimension ref="A1:L69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,15 +471,20 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
+          <t>relation_type</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
           <t>entity</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>answer_mid</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>relation_span</t>
         </is>
@@ -524,15 +529,20 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
+          <t>fb:medicine.drug_formulation.active_ingredients</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
           <t>what is the main ingredient in diamox sequels</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="K2" t="inlineStr">
         <is>
           <t>fb:m.0hqrhvc</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
+      <c r="L2" t="inlineStr">
         <is>
           <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -577,15 +587,20 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>&lt;UNK&gt;</t>
+          <t>fb:music.release_track.release</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
+          <t>&lt;UNK&gt;</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
           <t>fb:m.0qg9698</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr">
+      <c r="L3" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -630,15 +645,20 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>&lt;UNK&gt;</t>
+          <t>fb:common.topic.notable_types</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
+          <t>&lt;UNK&gt;</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
           <t>fb:m.0y9w_wv</t>
         </is>
       </c>
-      <c r="K4" t="inlineStr">
+      <c r="L4" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -683,15 +703,20 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>&lt;UNK&gt;</t>
+          <t>fb:tv.tv_program.genre</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
+          <t>&lt;UNK&gt;</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
           <t>fb:m.02ww_qc</t>
         </is>
       </c>
-      <c r="K5" t="inlineStr">
+      <c r="L5" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -736,15 +761,20 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>&lt;UNK&gt;</t>
+          <t>fb:film.producer.films_executive_produced</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
+          <t>&lt;UNK&gt;</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
           <t>fb:m.03yvtl5</t>
         </is>
       </c>
-      <c r="K6" t="inlineStr">
+      <c r="L6" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -789,15 +819,20 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>&lt;UNK&gt;</t>
+          <t>fb:music.album.album_content_type</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
+          <t>&lt;UNK&gt;</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
           <t>fb:m.01k0677</t>
         </is>
       </c>
-      <c r="K7" t="inlineStr">
+      <c r="L7" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -842,15 +877,20 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>&lt;UNK&gt;</t>
+          <t>fb:film.film.genre</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
+          <t>&lt;UNK&gt;</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
           <t>fb:m.0gw7q_r</t>
         </is>
       </c>
-      <c r="K8" t="inlineStr">
+      <c r="L8" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -895,15 +935,20 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>&lt;UNK&gt;</t>
+          <t>fb:business.company_type.companies_of_this_type</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
+          <t>&lt;UNK&gt;</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
           <t>fb:m.0319xp</t>
         </is>
       </c>
-      <c r="K9" t="inlineStr">
+      <c r="L9" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -948,15 +993,20 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>&lt;UNK&gt;</t>
+          <t>fb:people.person.place_of_birth</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
+          <t>&lt;UNK&gt;</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
           <t>fb:m.0jw1qp1</t>
         </is>
       </c>
-      <c r="K10" t="inlineStr">
+      <c r="L10" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -1001,15 +1051,20 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>&lt;UNK&gt;</t>
+          <t>fb:music.recording.canonical_version</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
+          <t>&lt;UNK&gt;</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
           <t>fb:m.0g71sbj</t>
         </is>
       </c>
-      <c r="K11" t="inlineStr">
+      <c r="L11" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -1054,15 +1109,20 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>&lt;UNK&gt;</t>
+          <t>fb:people.person.nationality</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
+          <t>&lt;UNK&gt;</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
           <t>fb:m.0z85h70</t>
         </is>
       </c>
-      <c r="K12" t="inlineStr">
+      <c r="L12" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -1107,15 +1167,20 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>&lt;UNK&gt;</t>
+          <t>fb:music.recording.artist</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
+          <t>&lt;UNK&gt;</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
           <t>fb:m.0nn66b_</t>
         </is>
       </c>
-      <c r="K13" t="inlineStr">
+      <c r="L13" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -1160,15 +1225,20 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>&lt;UNK&gt;</t>
+          <t>fb:music.album.album_content_type</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
+          <t>&lt;UNK&gt;</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
           <t>fb:m.0fr47rb</t>
         </is>
       </c>
-      <c r="K14" t="inlineStr">
+      <c r="L14" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -1213,15 +1283,20 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
+          <t>fb:medicine.drug_formulation.drug_category</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
           <t>is azolen</t>
         </is>
       </c>
-      <c r="J15" t="inlineStr">
+      <c r="K15" t="inlineStr">
         <is>
           <t>fb:m.0hqtlv8</t>
         </is>
       </c>
-      <c r="K15" t="inlineStr">
+      <c r="L15" t="inlineStr">
         <is>
           <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -1266,15 +1341,20 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>&lt;UNK&gt;</t>
+          <t>fb:music.album.album_content_type</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
+          <t>&lt;UNK&gt;</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
           <t>fb:m.0f8w6q8</t>
         </is>
       </c>
-      <c r="K16" t="inlineStr">
+      <c r="L16" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -1319,15 +1399,20 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
+          <t>fb:common.topic.notable_types</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
           <t>is abbe huc</t>
         </is>
       </c>
-      <c r="J17" t="inlineStr">
+      <c r="K17" t="inlineStr">
         <is>
           <t>fb:m.01wy9d</t>
         </is>
       </c>
-      <c r="K17" t="inlineStr">
+      <c r="L17" t="inlineStr">
         <is>
           <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -1372,15 +1457,20 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>&lt;UNK&gt;</t>
+          <t>fb:music.album.album_content_type</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
+          <t>&lt;UNK&gt;</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
           <t>fb:m.05ssss_</t>
         </is>
       </c>
-      <c r="K18" t="inlineStr">
+      <c r="L18" t="inlineStr">
         <is>
           <t>[0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -1425,15 +1515,20 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>&lt;UNK&gt;</t>
+          <t>fb:medicine.disease.causes</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
+          <t>&lt;UNK&gt;</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
           <t>fb:m.05n0276</t>
         </is>
       </c>
-      <c r="K19" t="inlineStr">
+      <c r="L19" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -1478,15 +1573,20 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>&lt;UNK&gt;</t>
+          <t>fb:people.profession.people_with_this_profession</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
+          <t>&lt;UNK&gt;</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
           <t>fb:m.02h664x</t>
         </is>
       </c>
-      <c r="K20" t="inlineStr">
+      <c r="L20" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -1531,15 +1631,20 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
+          <t>fb:medicine.drug_formulation.legal_status</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
           <t>what is the legal status of lomotil</t>
         </is>
       </c>
-      <c r="J21" t="inlineStr">
+      <c r="K21" t="inlineStr">
         <is>
           <t>fb:m.0hqr7sx</t>
         </is>
       </c>
-      <c r="K21" t="inlineStr">
+      <c r="L21" t="inlineStr">
         <is>
           <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -1584,15 +1689,20 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>&lt;UNK&gt;</t>
+          <t>fb:people.person.nationality</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
+          <t>&lt;UNK&gt;</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
           <t>fb:m.0j3wpr6</t>
         </is>
       </c>
-      <c r="K22" t="inlineStr">
+      <c r="L22" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -1637,15 +1747,20 @@
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>&lt;UNK&gt;</t>
+          <t>fb:music.album.artist</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
+          <t>&lt;UNK&gt;</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
           <t>fb:m.058mwwp</t>
         </is>
       </c>
-      <c r="K23" t="inlineStr">
+      <c r="L23" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -1690,15 +1805,20 @@
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>&lt;UNK&gt;</t>
+          <t>fb:film.film.genre</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
         <is>
+          <t>&lt;UNK&gt;</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
           <t>fb:m.0x17tvr</t>
         </is>
       </c>
-      <c r="K24" t="inlineStr">
+      <c r="L24" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -1743,15 +1863,20 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>&lt;UNK&gt;</t>
+          <t>fb:business.industry.companies</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
         <is>
+          <t>&lt;UNK&gt;</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
           <t>fb:m.02h7hyr</t>
         </is>
       </c>
-      <c r="K25" t="inlineStr">
+      <c r="L25" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -1796,15 +1921,20 @@
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>&lt;UNK&gt;</t>
+          <t>fb:music.recording.artist</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
         <is>
+          <t>&lt;UNK&gt;</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
           <t>fb:m.0zmpz4</t>
         </is>
       </c>
-      <c r="K26" t="inlineStr">
+      <c r="L26" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -1849,15 +1979,20 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>&lt;UNK&gt;</t>
+          <t>fb:music.release.track</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
         <is>
+          <t>&lt;UNK&gt;</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
           <t>fb:m.0g1vb16</t>
         </is>
       </c>
-      <c r="K27" t="inlineStr">
+      <c r="L27" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -1902,15 +2037,20 @@
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>&lt;UNK&gt;</t>
+          <t>fb:music.release.track</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
         <is>
+          <t>&lt;UNK&gt;</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
           <t>fb:m.033g8n3</t>
         </is>
       </c>
-      <c r="K28" t="inlineStr">
+      <c r="L28" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -1955,15 +2095,20 @@
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>&lt;UNK&gt;</t>
+          <t>fb:music.recording.artist</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
         <is>
+          <t>&lt;UNK&gt;</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
           <t>fb:m.0nm3chn</t>
         </is>
       </c>
-      <c r="K29" t="inlineStr">
+      <c r="L29" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -2008,15 +2153,20 @@
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>&lt;UNK&gt;</t>
+          <t>fb:fictional_universe.work_of_fiction.part_of_these_fictional_universes</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
         <is>
+          <t>&lt;UNK&gt;</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
           <t>fb:m.02qkdzb</t>
         </is>
       </c>
-      <c r="K30" t="inlineStr">
+      <c r="L30" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -2061,15 +2211,20 @@
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>&lt;UNK&gt;</t>
+          <t>fb:film.film.directed_by</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
         <is>
+          <t>&lt;UNK&gt;</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
           <t>fb:m.0b44bzz</t>
         </is>
       </c>
-      <c r="K31" t="inlineStr">
+      <c r="L31" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -2114,15 +2269,20 @@
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>&lt;UNK&gt;</t>
+          <t>fb:music.album.release_type</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
         <is>
+          <t>&lt;UNK&gt;</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
           <t>fb:m.07kg0mk</t>
         </is>
       </c>
-      <c r="K32" t="inlineStr">
+      <c r="L32" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -2167,15 +2327,20 @@
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>&lt;UNK&gt;</t>
+          <t>fb:music.recording.artist</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
         <is>
+          <t>&lt;UNK&gt;</t>
+        </is>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
           <t>fb:m.0d_bb4h</t>
         </is>
       </c>
-      <c r="K33" t="inlineStr">
+      <c r="L33" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -2220,15 +2385,20 @@
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>&lt;UNK&gt;</t>
+          <t>fb:music.recording.artist</t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
         <is>
+          <t>&lt;UNK&gt;</t>
+        </is>
+      </c>
+      <c r="K34" t="inlineStr">
+        <is>
           <t>fb:m.013f7rh</t>
         </is>
       </c>
-      <c r="K34" t="inlineStr">
+      <c r="L34" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -2273,15 +2443,20 @@
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>&lt;UNK&gt;</t>
+          <t>fb:music.release_track.release</t>
         </is>
       </c>
       <c r="J35" t="inlineStr">
         <is>
+          <t>&lt;UNK&gt;</t>
+        </is>
+      </c>
+      <c r="K35" t="inlineStr">
+        <is>
           <t>fb:m.0rtydgw</t>
         </is>
       </c>
-      <c r="K35" t="inlineStr">
+      <c r="L35" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -2326,15 +2501,20 @@
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>&lt;UNK&gt;</t>
+          <t>fb:american_football.football_player.position_s</t>
         </is>
       </c>
       <c r="J36" t="inlineStr">
         <is>
+          <t>&lt;UNK&gt;</t>
+        </is>
+      </c>
+      <c r="K36" t="inlineStr">
+        <is>
           <t>fb:m.0jbctxx</t>
         </is>
       </c>
-      <c r="K36" t="inlineStr">
+      <c r="L36" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -2379,15 +2559,20 @@
       </c>
       <c r="I37" t="inlineStr">
         <is>
+          <t>fb:medicine.drug_formulation.active_ingredients</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
           <t>active ingredient does presidents choice contain</t>
         </is>
       </c>
-      <c r="J37" t="inlineStr">
+      <c r="K37" t="inlineStr">
         <is>
           <t>fb:m.0hqskn0</t>
         </is>
       </c>
-      <c r="K37" t="inlineStr">
+      <c r="L37" t="inlineStr">
         <is>
           <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -2432,15 +2617,20 @@
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>&lt;UNK&gt;</t>
+          <t>fb:music.album.album_content_type</t>
         </is>
       </c>
       <c r="J38" t="inlineStr">
         <is>
+          <t>&lt;UNK&gt;</t>
+        </is>
+      </c>
+      <c r="K38" t="inlineStr">
+        <is>
           <t>fb:m.0f5n8xz</t>
         </is>
       </c>
-      <c r="K38" t="inlineStr">
+      <c r="L38" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -2485,15 +2675,20 @@
       </c>
       <c r="I39" t="inlineStr">
         <is>
+          <t>fb:cvg.cvg_platform.games_on_this_platform</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
           <t>'s a game on ti-99</t>
         </is>
       </c>
-      <c r="J39" t="inlineStr">
+      <c r="K39" t="inlineStr">
         <is>
           <t>fb:m.01pvj8</t>
         </is>
       </c>
-      <c r="K39" t="inlineStr">
+      <c r="L39" t="inlineStr">
         <is>
           <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -2538,15 +2733,20 @@
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>&lt;UNK&gt;</t>
+          <t>fb:people.profession.people_with_this_profession</t>
         </is>
       </c>
       <c r="J40" t="inlineStr">
         <is>
+          <t>&lt;UNK&gt;</t>
+        </is>
+      </c>
+      <c r="K40" t="inlineStr">
+        <is>
           <t>fb:m.02h664x</t>
         </is>
       </c>
-      <c r="K40" t="inlineStr">
+      <c r="L40" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -2591,15 +2791,20 @@
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>&lt;UNK&gt;</t>
+          <t>fb:film.film.country</t>
         </is>
       </c>
       <c r="J41" t="inlineStr">
         <is>
+          <t>&lt;UNK&gt;</t>
+        </is>
+      </c>
+      <c r="K41" t="inlineStr">
+        <is>
           <t>fb:m.0byd4y8</t>
         </is>
       </c>
-      <c r="K41" t="inlineStr">
+      <c r="L41" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -2644,15 +2849,20 @@
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>&lt;UNK&gt;</t>
+          <t>fb:music.release_track.release</t>
         </is>
       </c>
       <c r="J42" t="inlineStr">
         <is>
+          <t>&lt;UNK&gt;</t>
+        </is>
+      </c>
+      <c r="K42" t="inlineStr">
+        <is>
           <t>fb:m.0mkvdy4</t>
         </is>
       </c>
-      <c r="K42" t="inlineStr">
+      <c r="L42" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -2697,15 +2907,20 @@
       </c>
       <c r="I43" t="inlineStr">
         <is>
+          <t>fb:medicine.drug_formulation.drug_category</t>
+        </is>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
           <t>how would one categorize antacid antigas</t>
         </is>
       </c>
-      <c r="J43" t="inlineStr">
+      <c r="K43" t="inlineStr">
         <is>
           <t>fb:m.0hqrcx6</t>
         </is>
       </c>
-      <c r="K43" t="inlineStr">
+      <c r="L43" t="inlineStr">
         <is>
           <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -2750,15 +2965,20 @@
       </c>
       <c r="I44" t="inlineStr">
         <is>
+          <t>fb:base.pethealth.pet_disease_or_medical_condition.causes</t>
+        </is>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
           <t>causescanine parvovirus infection</t>
         </is>
       </c>
-      <c r="J44" t="inlineStr">
+      <c r="K44" t="inlineStr">
         <is>
           <t>fb:m.05dbwcp</t>
         </is>
       </c>
-      <c r="K44" t="inlineStr">
+      <c r="L44" t="inlineStr">
         <is>
           <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -2803,15 +3023,20 @@
       </c>
       <c r="I45" t="inlineStr">
         <is>
+          <t>fb:medicine.drug_formulation.legal_status</t>
+        </is>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
           <t>what is suphedrine pe</t>
         </is>
       </c>
-      <c r="J45" t="inlineStr">
+      <c r="K45" t="inlineStr">
         <is>
           <t>fb:m.0hqrs1d</t>
         </is>
       </c>
-      <c r="K45" t="inlineStr">
+      <c r="L45" t="inlineStr">
         <is>
           <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -2856,15 +3081,20 @@
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>&lt;UNK&gt;</t>
+          <t>fb:user.mt.default_domain.metabolite.associated_disorder</t>
         </is>
       </c>
       <c r="J46" t="inlineStr">
         <is>
+          <t>&lt;UNK&gt;</t>
+        </is>
+      </c>
+      <c r="K46" t="inlineStr">
+        <is>
           <t>fb:m.02kc1x8</t>
         </is>
       </c>
-      <c r="K46" t="inlineStr">
+      <c r="L46" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -2909,15 +3139,20 @@
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>&lt;UNK&gt;</t>
+          <t>fb:people.profession.people_with_this_profession</t>
         </is>
       </c>
       <c r="J47" t="inlineStr">
         <is>
+          <t>&lt;UNK&gt;</t>
+        </is>
+      </c>
+      <c r="K47" t="inlineStr">
+        <is>
           <t>fb:m.02h664x</t>
         </is>
       </c>
-      <c r="K47" t="inlineStr">
+      <c r="L47" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -2962,15 +3197,20 @@
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>&lt;UNK&gt;</t>
+          <t>fb:people.deceased_person.place_of_death</t>
         </is>
       </c>
       <c r="J48" t="inlineStr">
         <is>
+          <t>&lt;UNK&gt;</t>
+        </is>
+      </c>
+      <c r="K48" t="inlineStr">
+        <is>
           <t>fb:m.0zgl46r</t>
         </is>
       </c>
-      <c r="K48" t="inlineStr">
+      <c r="L48" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -3015,15 +3255,20 @@
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>&lt;UNK&gt;</t>
+          <t>fb:tv.tv_series_episode.series</t>
         </is>
       </c>
       <c r="J49" t="inlineStr">
         <is>
+          <t>&lt;UNK&gt;</t>
+        </is>
+      </c>
+      <c r="K49" t="inlineStr">
+        <is>
           <t>fb:m.0kpck1k</t>
         </is>
       </c>
-      <c r="K49" t="inlineStr">
+      <c r="L49" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -3068,15 +3313,20 @@
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>&lt;UNK&gt;</t>
+          <t>fb:music.composition.lyricist</t>
         </is>
       </c>
       <c r="J50" t="inlineStr">
         <is>
+          <t>&lt;UNK&gt;</t>
+        </is>
+      </c>
+      <c r="K50" t="inlineStr">
+        <is>
           <t>fb:m.0_jqh5j</t>
         </is>
       </c>
-      <c r="K50" t="inlineStr">
+      <c r="L50" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -3121,15 +3371,20 @@
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>&lt;UNK&gt;</t>
+          <t>fb:music.release_track.release</t>
         </is>
       </c>
       <c r="J51" t="inlineStr">
         <is>
+          <t>&lt;UNK&gt;</t>
+        </is>
+      </c>
+      <c r="K51" t="inlineStr">
+        <is>
           <t>fb:m.0km51t_</t>
         </is>
       </c>
-      <c r="K51" t="inlineStr">
+      <c r="L51" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -3174,15 +3429,20 @@
       </c>
       <c r="I52" t="inlineStr">
         <is>
-          <t>&lt;UNK&gt;</t>
+          <t>fb:music.release_track.release</t>
         </is>
       </c>
       <c r="J52" t="inlineStr">
         <is>
+          <t>&lt;UNK&gt;</t>
+        </is>
+      </c>
+      <c r="K52" t="inlineStr">
+        <is>
           <t>fb:m.0v48dg8</t>
         </is>
       </c>
-      <c r="K52" t="inlineStr">
+      <c r="L52" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -3227,15 +3487,20 @@
       </c>
       <c r="I53" t="inlineStr">
         <is>
+          <t>fb:medicine.drug_formulation.drug_category</t>
+        </is>
+      </c>
+      <c r="J53" t="inlineStr">
+        <is>
           <t>is humatrope ?</t>
         </is>
       </c>
-      <c r="J53" t="inlineStr">
+      <c r="K53" t="inlineStr">
         <is>
           <t>fb:m.0hqth1v</t>
         </is>
       </c>
-      <c r="K53" t="inlineStr">
+      <c r="L53" t="inlineStr">
         <is>
           <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -3280,15 +3545,20 @@
       </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t>&lt;UNK&gt;</t>
+          <t>fb:tv.tv_series_episode.series</t>
         </is>
       </c>
       <c r="J54" t="inlineStr">
         <is>
+          <t>&lt;UNK&gt;</t>
+        </is>
+      </c>
+      <c r="K54" t="inlineStr">
+        <is>
           <t>fb:m.0k33swc</t>
         </is>
       </c>
-      <c r="K54" t="inlineStr">
+      <c r="L54" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -3333,15 +3603,20 @@
       </c>
       <c r="I55" t="inlineStr">
         <is>
-          <t>&lt;UNK&gt;</t>
+          <t>fb:book.written_work.author</t>
         </is>
       </c>
       <c r="J55" t="inlineStr">
         <is>
+          <t>&lt;UNK&gt;</t>
+        </is>
+      </c>
+      <c r="K55" t="inlineStr">
+        <is>
           <t>fb:m.06hsptf</t>
         </is>
       </c>
-      <c r="K55" t="inlineStr">
+      <c r="L55" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -3386,15 +3661,20 @@
       </c>
       <c r="I56" t="inlineStr">
         <is>
-          <t>&lt;UNK&gt;</t>
+          <t>fb:book.written_work.author</t>
         </is>
       </c>
       <c r="J56" t="inlineStr">
         <is>
+          <t>&lt;UNK&gt;</t>
+        </is>
+      </c>
+      <c r="K56" t="inlineStr">
+        <is>
           <t>fb:m.04w2yxm</t>
         </is>
       </c>
-      <c r="K56" t="inlineStr">
+      <c r="L56" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -3439,15 +3719,20 @@
       </c>
       <c r="I57" t="inlineStr">
         <is>
+          <t>fb:base.rugby.rugby_player.type_of_rugby</t>
+        </is>
+      </c>
+      <c r="J57" t="inlineStr">
+        <is>
           <t>what</t>
         </is>
       </c>
-      <c r="J57" t="inlineStr">
+      <c r="K57" t="inlineStr">
         <is>
           <t>fb:m.05h4n_p</t>
         </is>
       </c>
-      <c r="K57" t="inlineStr">
+      <c r="L57" t="inlineStr">
         <is>
           <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -3492,15 +3777,20 @@
       </c>
       <c r="I58" t="inlineStr">
         <is>
-          <t>&lt;UNK&gt;</t>
+          <t>fb:music.recording.releases</t>
         </is>
       </c>
       <c r="J58" t="inlineStr">
         <is>
+          <t>&lt;UNK&gt;</t>
+        </is>
+      </c>
+      <c r="K58" t="inlineStr">
+        <is>
           <t>fb:m.0r4l5d</t>
         </is>
       </c>
-      <c r="K58" t="inlineStr">
+      <c r="L58" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -3545,15 +3835,20 @@
       </c>
       <c r="I59" t="inlineStr">
         <is>
-          <t>&lt;UNK&gt;</t>
+          <t>fb:music.album.artist</t>
         </is>
       </c>
       <c r="J59" t="inlineStr">
         <is>
+          <t>&lt;UNK&gt;</t>
+        </is>
+      </c>
+      <c r="K59" t="inlineStr">
+        <is>
           <t>fb:m.0fjg6cy</t>
         </is>
       </c>
-      <c r="K59" t="inlineStr">
+      <c r="L59" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -3598,15 +3893,20 @@
       </c>
       <c r="I60" t="inlineStr">
         <is>
-          <t>&lt;UNK&gt;</t>
+          <t>fb:people.person.gender</t>
         </is>
       </c>
       <c r="J60" t="inlineStr">
         <is>
+          <t>&lt;UNK&gt;</t>
+        </is>
+      </c>
+      <c r="K60" t="inlineStr">
+        <is>
           <t>fb:m.0h81j6h</t>
         </is>
       </c>
-      <c r="K60" t="inlineStr">
+      <c r="L60" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -3651,15 +3951,20 @@
       </c>
       <c r="I61" t="inlineStr">
         <is>
-          <t>&lt;UNK&gt;</t>
+          <t>fb:user.mt.default_domain.biofunction.metabolites</t>
         </is>
       </c>
       <c r="J61" t="inlineStr">
         <is>
+          <t>&lt;UNK&gt;</t>
+        </is>
+      </c>
+      <c r="K61" t="inlineStr">
+        <is>
           <t>fb:m.02kbxdm</t>
         </is>
       </c>
-      <c r="K61" t="inlineStr">
+      <c r="L61" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -3704,15 +4009,20 @@
       </c>
       <c r="I62" t="inlineStr">
         <is>
-          <t>&lt;UNK&gt;</t>
+          <t>fb:people.person.nationality</t>
         </is>
       </c>
       <c r="J62" t="inlineStr">
         <is>
+          <t>&lt;UNK&gt;</t>
+        </is>
+      </c>
+      <c r="K62" t="inlineStr">
+        <is>
           <t>fb:m.0cz7_3h</t>
         </is>
       </c>
-      <c r="K62" t="inlineStr">
+      <c r="L62" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -3757,15 +4067,20 @@
       </c>
       <c r="I63" t="inlineStr">
         <is>
+          <t>fb:music.album.artist</t>
+        </is>
+      </c>
+      <c r="J63" t="inlineStr">
+        <is>
           <t>who released the album jerusalem</t>
         </is>
       </c>
-      <c r="J63" t="inlineStr">
+      <c r="K63" t="inlineStr">
         <is>
           <t>fb:m.01k5hzy</t>
         </is>
       </c>
-      <c r="K63" t="inlineStr">
+      <c r="L63" t="inlineStr">
         <is>
           <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -3810,15 +4125,20 @@
       </c>
       <c r="I64" t="inlineStr">
         <is>
-          <t>&lt;UNK&gt;</t>
+          <t>fb:cvg.computer_videogame.gameplay_modes</t>
         </is>
       </c>
       <c r="J64" t="inlineStr">
         <is>
+          <t>&lt;UNK&gt;</t>
+        </is>
+      </c>
+      <c r="K64" t="inlineStr">
+        <is>
           <t>fb:m.06k50f</t>
         </is>
       </c>
-      <c r="K64" t="inlineStr">
+      <c r="L64" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -3863,15 +4183,20 @@
       </c>
       <c r="I65" t="inlineStr">
         <is>
-          <t>&lt;UNK&gt;</t>
+          <t>fb:music.release_track.release</t>
         </is>
       </c>
       <c r="J65" t="inlineStr">
         <is>
+          <t>&lt;UNK&gt;</t>
+        </is>
+      </c>
+      <c r="K65" t="inlineStr">
+        <is>
           <t>fb:m.0ls67qg</t>
         </is>
       </c>
-      <c r="K65" t="inlineStr">
+      <c r="L65" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -3916,15 +4241,20 @@
       </c>
       <c r="I66" t="inlineStr">
         <is>
-          <t>&lt;UNK&gt;</t>
+          <t>fb:music.artist.track</t>
         </is>
       </c>
       <c r="J66" t="inlineStr">
         <is>
+          <t>&lt;UNK&gt;</t>
+        </is>
+      </c>
+      <c r="K66" t="inlineStr">
+        <is>
           <t>fb:m.01npl51</t>
         </is>
       </c>
-      <c r="K66" t="inlineStr">
+      <c r="L66" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -3969,15 +4299,20 @@
       </c>
       <c r="I67" t="inlineStr">
         <is>
+          <t>fb:music.album.artist</t>
+        </is>
+      </c>
+      <c r="J67" t="inlineStr">
+        <is>
           <t>artist released the album</t>
         </is>
       </c>
-      <c r="J67" t="inlineStr">
+      <c r="K67" t="inlineStr">
         <is>
           <t>fb:m.03jhpgp</t>
         </is>
       </c>
-      <c r="K67" t="inlineStr">
+      <c r="L67" t="inlineStr">
         <is>
           <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -4022,15 +4357,20 @@
       </c>
       <c r="I68" t="inlineStr">
         <is>
+          <t>fb:medicine.drug_formulation.drug_category</t>
+        </is>
+      </c>
+      <c r="J68" t="inlineStr">
+        <is>
           <t>what is tonojug</t>
         </is>
       </c>
-      <c r="J68" t="inlineStr">
+      <c r="K68" t="inlineStr">
         <is>
           <t>fb:m.0hqv1cb</t>
         </is>
       </c>
-      <c r="K68" t="inlineStr">
+      <c r="L68" t="inlineStr">
         <is>
           <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
@@ -4075,15 +4415,20 @@
       </c>
       <c r="I69" t="inlineStr">
         <is>
-          <t>&lt;UNK&gt;</t>
+          <t>fb:music.artist.genre</t>
         </is>
       </c>
       <c r="J69" t="inlineStr">
         <is>
+          <t>&lt;UNK&gt;</t>
+        </is>
+      </c>
+      <c r="K69" t="inlineStr">
+        <is>
           <t>fb:m.04634rs</t>
         </is>
       </c>
-      <c r="K69" t="inlineStr">
+      <c r="L69" t="inlineStr">
         <is>
           <t>[0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>

</xml_diff>